<commit_message>
Updated log with new iteration of the system
</commit_message>
<xml_diff>
--- a/output/predictions__C2mim__CH3SO3__Aluminum_Oxide__Al2O3__50_0_10_0_-.xlsx
+++ b/output/predictions__C2mim__CH3SO3__Aluminum_Oxide__Al2O3__50_0_10_0_-.xlsx
@@ -504,7 +504,7 @@
         <v>0.202699276</v>
       </c>
       <c r="H2" t="n">
-        <v>0.2016236484050751</v>
+        <v>0.2014809846878052</v>
       </c>
     </row>
     <row r="3">
@@ -536,7 +536,7 @@
         <v>0.203122119</v>
       </c>
       <c r="H3" t="n">
-        <v>0.201588362455368</v>
+        <v>0.201513260602951</v>
       </c>
     </row>
     <row r="4">
@@ -568,7 +568,7 @@
         <v>0.201385065</v>
       </c>
       <c r="H4" t="n">
-        <v>0.2015264332294464</v>
+        <v>0.2014876157045364</v>
       </c>
     </row>
     <row r="5">
@@ -600,7 +600,7 @@
         <v>0.201440124</v>
       </c>
       <c r="H5" t="n">
-        <v>0.2013671547174454</v>
+        <v>0.2012569904327393</v>
       </c>
     </row>
     <row r="6">
@@ -632,7 +632,7 @@
         <v>0.201043858</v>
       </c>
       <c r="H6" t="n">
-        <v>0.2008635848760605</v>
+        <v>0.2008634060621262</v>
       </c>
     </row>
     <row r="7">
@@ -664,7 +664,7 @@
         <v>0.200029423</v>
       </c>
       <c r="H7" t="n">
-        <v>0.2003562450408936</v>
+        <v>0.2003986388444901</v>
       </c>
     </row>
   </sheetData>

</xml_diff>